<commit_message>
designed ml experiment structure
</commit_message>
<xml_diff>
--- a/data_acquisition/wing_leakage_data_samples_filt.xlsx
+++ b/data_acquisition/wing_leakage_data_samples_filt.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="43">
   <si>
     <t xml:space="preserve">sample_number</t>
   </si>
@@ -139,6 +139,9 @@
     <t xml:space="preserve">residual flow of 0.010 in mfc7 and 0.0173 in mfc10</t>
   </si>
   <si>
+    <t xml:space="preserve">missed</t>
+  </si>
+  <si>
     <t xml:space="preserve">observed residual leakage of 0.0167 in mfc10</t>
   </si>
   <si>
@@ -155,7 +158,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -183,11 +186,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -259,16 +257,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -350,8 +348,8 @@
   </sheetPr>
   <dimension ref="A1:S2007"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1965" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2003" activeCellId="0" sqref="A2003"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A697" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q712" activeCellId="0" sqref="Q712"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24482,6 +24480,9 @@
         <f aca="false">SUM(F523:O523)</f>
         <v>0</v>
       </c>
+      <c r="Q523" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="R523" s="1" t="n">
         <v>8</v>
       </c>
@@ -24870,7 +24871,7 @@
         <v>0.38</v>
       </c>
       <c r="Q534" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="R534" s="1" t="n">
         <v>9</v>
@@ -24949,7 +24950,7 @@
       <c r="F536" s="1" t="n">
         <v>0.0459</v>
       </c>
-      <c r="G536" s="5" t="n">
+      <c r="G536" s="6" t="n">
         <v>0.0537</v>
       </c>
       <c r="H536" s="1" t="n">
@@ -30057,7 +30058,7 @@
         <v>0.6714</v>
       </c>
       <c r="Q655" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="R655" s="1" t="n">
         <v>10</v>
@@ -32444,6 +32445,9 @@
         <f aca="false">SUM(F709:O709)</f>
         <v>0</v>
       </c>
+      <c r="Q709" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="R709" s="1" t="n">
         <v>10</v>
       </c>
@@ -32489,6 +32493,9 @@
         <f aca="false">SUM(F711:O711)</f>
         <v>0</v>
       </c>
+      <c r="Q711" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="R711" s="1" t="n">
         <v>10</v>
       </c>
@@ -34224,7 +34231,7 @@
         <v>0.3298</v>
       </c>
       <c r="Q748" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R748" s="1" t="n">
         <v>11</v>
@@ -61933,10 +61940,10 @@
       <c r="C2002" s="1" t="n">
         <v>2100</v>
       </c>
-      <c r="D2002" s="6" t="n">
+      <c r="D2002" s="7" t="n">
         <v>14680</v>
       </c>
-      <c r="E2002" s="7" t="n">
+      <c r="E2002" s="6" t="n">
         <v>3350</v>
       </c>
       <c r="F2002" s="1" t="n">
@@ -62032,8 +62039,8 @@
       </c>
     </row>
     <row r="2007" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D2007" s="6"/>
-      <c r="E2007" s="7"/>
+      <c r="D2007" s="7"/>
+      <c r="E2007" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>